<commit_message>
Update manage avvisi in rest api
- Added Endpoints:
/avviso/segna-come-letto/{id_avviso}
/avviso/segna-come-nascosto/{id_avviso}
/avviso/crea
</commit_message>
<xml_diff>
--- a/completezza funzionale.xlsx
+++ b/completezza funzionale.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salvc\Desktop\Ratatouille23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7620B0-27A5-47CD-9121-785935A60D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F22129-9A92-4E36-801C-06A7FD10ADB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3135" yWindow="1035" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Funzionalità #1</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Signup Requests</t>
   </si>
   <si>
-    <t>setAvvisoViewed #incompleto</t>
-  </si>
-  <si>
     <t>/avvisi-viewed/{id_user}</t>
   </si>
   <si>
@@ -136,13 +133,22 @@
   </si>
   <si>
     <t>/avvisi?id_ristorante=</t>
+  </si>
+  <si>
+    <t>/avviso/crea</t>
+  </si>
+  <si>
+    <t>/avviso/segna-come-letto/{id_avviso}</t>
+  </si>
+  <si>
+    <t>/avviso/segna-come-nascosto/{id_avviso}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +170,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -340,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -623,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,14 +700,17 @@
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>33</v>
+      <c r="B3" t="s">
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -703,11 +720,11 @@
       <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>35</v>
+      <c r="D4" t="s">
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -715,7 +732,7 @@
         <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -723,7 +740,7 @@
         <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -731,13 +748,16 @@
         <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -748,6 +768,7 @@
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">

</xml_diff>